<commit_message>
recalculated the SD, edited df/SD table
</commit_message>
<xml_diff>
--- a/dand_1_test_a_perceptual_phenomenon/p1_test_a_perceptual_phenomenon_data.xlsx
+++ b/dand_1_test_a_perceptual_phenomenon/p1_test_a_perceptual_phenomenon_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ltelwest/Google Drive/Data Science/Udacity/Data Analyst/Problemset 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lt/Git/udacity-projects/dand_1_test_a_perceptual_phenomenon/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="stroopdata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Congruent</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>-&gt; 48% of the differences in time taken for the quiz are due to congruent vs. incongruent</t>
+  </si>
+  <si>
+    <t>Standard error calc</t>
+  </si>
+  <si>
+    <t>Congruent - Mean</t>
+  </si>
+  <si>
+    <t>Squared</t>
   </si>
 </sst>
 </file>
@@ -88,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -130,12 +139,92 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -165,26 +254,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="24">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -196,8 +294,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Prozent" xfId="21" builtinId="5"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="21" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -472,388 +570,831 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:E18"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="E1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
         <v>12.079000000000001</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
+        <f>A2-AVERAGE($A$2:$A$25)</f>
+        <v>-1.9721250000000001</v>
+      </c>
+      <c r="C2" s="11">
+        <f>B2^2</f>
+        <v>3.8892770156250007</v>
+      </c>
+      <c r="D2" s="10">
         <v>19.277999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="E2" s="6">
+        <f>D2-AVERAGE($D$2:$D$25)</f>
+        <v>-2.7379166666666706</v>
+      </c>
+      <c r="F2" s="11">
+        <f>E2^2</f>
+        <v>7.4961876736111321</v>
+      </c>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
         <v>16.791</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B25" si="0">A3-AVERAGE($A$2:$A$25)</f>
+        <v>2.7398749999999996</v>
+      </c>
+      <c r="C3" s="11">
+        <f t="shared" ref="C3:C25" si="1">B3^2</f>
+        <v>7.5069150156249975</v>
+      </c>
+      <c r="D3" s="10">
         <v>18.741</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E25" si="2">D3-AVERAGE($D$2:$D$25)</f>
+        <v>-3.2749166666666696</v>
+      </c>
+      <c r="F3" s="11">
+        <f t="shared" ref="F3:F25" si="3">E3^2</f>
+        <v>10.72507917361113</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
         <v>9.5640000000000001</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
+        <f t="shared" si="0"/>
+        <v>-4.4871250000000007</v>
+      </c>
+      <c r="C4" s="11">
+        <f t="shared" si="1"/>
+        <v>20.134290765625007</v>
+      </c>
+      <c r="D4" s="10">
         <v>21.213999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="E4" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.80191666666667061</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" si="3"/>
+        <v>0.64307034027778409</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
         <v>8.6300000000000008</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+        <v>-5.421125</v>
+      </c>
+      <c r="C5" s="11">
+        <f t="shared" si="1"/>
+        <v>29.388596265625001</v>
+      </c>
+      <c r="D5" s="10">
         <v>15.686999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="E5" s="6">
+        <f t="shared" si="2"/>
+        <v>-6.3289166666666699</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="3"/>
+        <v>40.055186173611155</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
         <v>14.669</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.61787499999999973</v>
+      </c>
+      <c r="C6" s="11">
+        <f t="shared" si="1"/>
+        <v>0.38176951562499967</v>
+      </c>
+      <c r="D6" s="10">
         <v>22.803000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="E6" s="6">
+        <f t="shared" si="2"/>
+        <v>0.78708333333333158</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="3"/>
+        <v>0.61950017361110832</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
         <v>12.238</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.8131250000000012</v>
+      </c>
+      <c r="C7" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2874222656250045</v>
+      </c>
+      <c r="D7" s="10">
         <v>20.878</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="E7" s="6">
+        <f t="shared" si="2"/>
+        <v>-1.1379166666666691</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="3"/>
+        <v>1.2948543402777835</v>
+      </c>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
         <v>14.692</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.64087499999999942</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="1"/>
+        <v>0.41072076562499926</v>
+      </c>
+      <c r="D8" s="10">
         <v>24.571999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="E8" s="6">
+        <f t="shared" si="2"/>
+        <v>2.5560833333333299</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="3"/>
+        <v>6.5335620069444271</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
         <v>8.9870000000000001</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="6">
+        <f t="shared" si="0"/>
+        <v>-5.0641250000000007</v>
+      </c>
+      <c r="C9" s="11">
+        <f t="shared" si="1"/>
+        <v>25.645362015625008</v>
+      </c>
+      <c r="D9" s="10">
         <v>17.393999999999998</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6">
+        <f t="shared" si="2"/>
+        <v>-4.6219166666666709</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="3"/>
+        <v>21.362113673611152</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="I9" t="s">
         <v>0</v>
       </c>
-      <c r="F9" t="s">
+      <c r="J9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
         <v>9.4009999999999998</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
+        <f t="shared" si="0"/>
+        <v>-4.650125000000001</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="1"/>
+        <v>21.623662515625011</v>
+      </c>
+      <c r="D10" s="10">
         <v>20.762</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="6">
+        <f t="shared" si="2"/>
+        <v>-1.2539166666666688</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="3"/>
+        <v>1.5723070069444498</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" t="s">
         <v>2</v>
       </c>
-      <c r="E10">
+      <c r="I10">
         <f>COUNT(A2:A25)</f>
         <v>24</v>
       </c>
-      <c r="F10">
-        <f>COUNT(B2:B25)</f>
+      <c r="J10">
+        <f>COUNT(D2:D25)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
         <v>14.48</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="6">
+        <f t="shared" si="0"/>
+        <v>0.42887499999999967</v>
+      </c>
+      <c r="C11" s="11">
+        <f t="shared" si="1"/>
+        <v>0.18393376562499972</v>
+      </c>
+      <c r="D11" s="10">
         <v>26.282</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="6">
+        <f t="shared" si="2"/>
+        <v>4.2660833333333308</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="3"/>
+        <v>18.199467006944424</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="1">
+      <c r="I11" s="1">
         <f>MIN(A2:A25)</f>
         <v>8.6300000000000008</v>
       </c>
-      <c r="F11" s="1">
-        <f>MIN(B2:B25)</f>
+      <c r="J11" s="1">
+        <f>MIN(D2:D25)</f>
         <v>15.686999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
         <v>22.327999999999999</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="6">
+        <f t="shared" si="0"/>
+        <v>8.2768749999999986</v>
+      </c>
+      <c r="C12" s="11">
+        <f t="shared" si="1"/>
+        <v>68.506659765624974</v>
+      </c>
+      <c r="D12" s="10">
         <v>24.524000000000001</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="6">
+        <f t="shared" si="2"/>
+        <v>2.5080833333333317</v>
+      </c>
+      <c r="F12" s="11">
+        <f t="shared" si="3"/>
+        <v>6.290482006944436</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="1">
+      <c r="I12" s="1">
         <f>_xlfn.PERCENTILE.INC(A2:A25,0.25)</f>
         <v>11.895250000000001</v>
       </c>
-      <c r="F12" s="1">
-        <f>_xlfn.PERCENTILE.INC(B2:B25,0.25)</f>
+      <c r="J12" s="1">
+        <f>_xlfn.PERCENTILE.INC(D2:D25,0.25)</f>
         <v>18.716749999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
         <v>15.298</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2468749999999993</v>
+      </c>
+      <c r="C13" s="11">
+        <f t="shared" si="1"/>
+        <v>1.5546972656249982</v>
+      </c>
+      <c r="D13" s="10">
         <v>18.643999999999998</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="6">
+        <f t="shared" si="2"/>
+        <v>-3.3719166666666709</v>
+      </c>
+      <c r="F13" s="11">
+        <f t="shared" si="3"/>
+        <v>11.369822006944473</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="1">
+      <c r="I13" s="1">
         <f>MEDIAN(A2:A25)</f>
         <v>14.3565</v>
       </c>
-      <c r="F13" s="1">
-        <f>MEDIAN(B2:B25)</f>
+      <c r="J13" s="1">
+        <f>MEDIAN(D2:D25)</f>
         <v>21.017499999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
         <v>15.073</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0218749999999996</v>
+      </c>
+      <c r="C14" s="11">
+        <f t="shared" si="1"/>
+        <v>1.0442285156249993</v>
+      </c>
+      <c r="D14" s="10">
         <v>17.510000000000002</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="6">
+        <f t="shared" si="2"/>
+        <v>-4.5059166666666677</v>
+      </c>
+      <c r="F14" s="11">
+        <f t="shared" si="3"/>
+        <v>20.303285006944453</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="1">
+      <c r="I14" s="1">
         <f>_xlfn.PERCENTILE.INC(A2:A25,0.75)</f>
         <v>16.200749999999999</v>
       </c>
-      <c r="F14" s="1">
-        <f>_xlfn.PERCENTILE.INC(B2:B25,0.75)</f>
+      <c r="J14" s="1">
+        <f>_xlfn.PERCENTILE.INC(D2:D25,0.75)</f>
         <v>24.051499999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
         <v>16.928999999999998</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="6">
+        <f t="shared" si="0"/>
+        <v>2.8778749999999977</v>
+      </c>
+      <c r="C15" s="11">
+        <f t="shared" si="1"/>
+        <v>8.2821645156249861</v>
+      </c>
+      <c r="D15" s="10">
         <v>20.329999999999998</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="6">
+        <f t="shared" si="2"/>
+        <v>-1.6859166666666709</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" si="3"/>
+        <v>2.8423150069444589</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="1">
-        <f>AVERAGE(A2:B25)</f>
-        <v>18.033520833333334</v>
-      </c>
-      <c r="F15" s="1">
-        <f>AVERAGE(B2:C25)</f>
-        <v>22.015916666666669</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="I15" s="1">
+        <f>AVERAGE(A2:D25)</f>
+        <v>12.052048631510418</v>
+      </c>
+      <c r="J15" s="1">
+        <f>AVERAGE(D2:E25)</f>
+        <v>11.007958333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
         <v>18.2</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1488749999999985</v>
+      </c>
+      <c r="C16" s="11">
+        <f t="shared" si="1"/>
+        <v>17.213163765624987</v>
+      </c>
+      <c r="D16" s="10">
         <v>35.255000000000003</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="6">
+        <f t="shared" si="2"/>
+        <v>13.239083333333333</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" si="3"/>
+        <v>175.27332750694444</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="1">
+      <c r="I16" s="1">
         <f>MAX(A2:A25)</f>
         <v>22.327999999999999</v>
       </c>
-      <c r="F16" s="1">
-        <f>MAX(B2:B25)</f>
+      <c r="J16" s="1">
+        <f>MAX(D2:D25)</f>
         <v>35.255000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
         <v>12.13</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.921125</v>
+      </c>
+      <c r="C17" s="11">
+        <f t="shared" si="1"/>
+        <v>3.6907212656249997</v>
+      </c>
+      <c r="D17" s="10">
         <v>22.158000000000001</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="6">
+        <f t="shared" si="2"/>
+        <v>0.14208333333333201</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="3"/>
+        <v>2.0187673611110735E-2</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="1">
+      <c r="I17" s="1">
         <f>VARA(A2:A25)</f>
         <v>12.669029070652117</v>
       </c>
-      <c r="F17" s="1">
-        <f>VARA(B2:B25)</f>
+      <c r="J17" s="1">
+        <f>VARA(D2:D25)</f>
         <v>23.011757036231874</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
         <v>18.495000000000001</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="6">
+        <f t="shared" si="0"/>
+        <v>4.4438750000000002</v>
+      </c>
+      <c r="C18" s="11">
+        <f t="shared" si="1"/>
+        <v>19.748025015625004</v>
+      </c>
+      <c r="D18" s="10">
         <v>25.138999999999999</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" s="6">
+        <f t="shared" si="2"/>
+        <v>3.1230833333333301</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" si="3"/>
+        <v>9.7536495069444236</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="1">
-        <f>_xlfn.STDEV.P(A2:A25)</f>
-        <v>3.4844157127666247</v>
-      </c>
-      <c r="F18" s="1">
-        <f>_xlfn.STDEV.P(B2:B25)</f>
-        <v>4.6960551345133137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="I18" s="1">
+        <f>STDEV(A2:A25)</f>
+        <v>3.559357957645187</v>
+      </c>
+      <c r="J18" s="1">
+        <f>STDEV(D2:D25)</f>
+        <v>4.7970571224691367</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
         <v>10.638999999999999</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="6">
+        <f t="shared" si="0"/>
+        <v>-3.4121250000000014</v>
+      </c>
+      <c r="C19" s="11">
+        <f t="shared" si="1"/>
+        <v>11.642597015625009</v>
+      </c>
+      <c r="D19" s="10">
         <v>20.428999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="E19" s="6">
+        <f t="shared" si="2"/>
+        <v>-1.5869166666666707</v>
+      </c>
+      <c r="F19" s="11">
+        <f t="shared" si="3"/>
+        <v>2.5183045069444576</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="1">
+        <f>SQRT(SUM(C2:C25)/(COUNT(C2:C25)-1))</f>
+        <v>3.5593579576451955</v>
+      </c>
+      <c r="J19" s="1">
+        <f>SQRT(SUM(D2:D25)/(COUNT(D2:D25)-1))</f>
+        <v>4.7930293588483899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
         <v>11.343999999999999</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="6">
+        <f t="shared" si="0"/>
+        <v>-2.7071250000000013</v>
+      </c>
+      <c r="C20" s="11">
+        <f t="shared" si="1"/>
+        <v>7.3285257656250069</v>
+      </c>
+      <c r="D20" s="10">
         <v>17.425000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="E20" s="6">
+        <f t="shared" si="2"/>
+        <v>-4.5909166666666685</v>
+      </c>
+      <c r="F20" s="11">
+        <f t="shared" si="3"/>
+        <v>21.076515840277796</v>
+      </c>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
         <v>12.369</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.682125000000001</v>
+      </c>
+      <c r="C21" s="11">
+        <f t="shared" si="1"/>
+        <v>2.8295445156250034</v>
+      </c>
+      <c r="D21" s="10">
         <v>34.287999999999997</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" s="6">
+        <f t="shared" si="2"/>
+        <v>12.272083333333327</v>
+      </c>
+      <c r="F21" s="11">
+        <f t="shared" si="3"/>
+        <v>150.60402934027763</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="3">
-        <f>SQRT(E18^2/24+F18^2/24)</f>
-        <v>1.1936304335542156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="I21" s="3">
+        <f>SQRT(I18^2/24+J18^2/24)</f>
+        <v>1.2193028422505077</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
         <v>12.944000000000001</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.1071249999999999</v>
+      </c>
+      <c r="C22" s="11">
+        <f t="shared" si="1"/>
+        <v>1.2257257656249998</v>
+      </c>
+      <c r="D22" s="10">
         <v>23.893999999999998</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8780833333333291</v>
+      </c>
+      <c r="F22" s="11">
+        <f t="shared" si="3"/>
+        <v>3.5271970069444287</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="5">
-        <f>COUNT(A2:A25)+COUNT(B2:B25)-2</f>
+      <c r="I22" s="5">
+        <f>COUNT(A2:A25)+COUNT(D2:D25)-2</f>
         <v>46</v>
       </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
         <v>14.233000000000001</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="6">
+        <f t="shared" si="0"/>
+        <v>0.18187499999999979</v>
+      </c>
+      <c r="C23" s="11">
+        <f t="shared" si="1"/>
+        <v>3.3078515624999923E-2</v>
+      </c>
+      <c r="D23" s="10">
         <v>17.96</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" s="6">
+        <f t="shared" si="2"/>
+        <v>-4.0559166666666684</v>
+      </c>
+      <c r="F23" s="11">
+        <f t="shared" si="3"/>
+        <v>16.450460006944457</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="3">
+      <c r="I23" s="3">
         <v>3.496</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
         <v>19.71</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="6">
+        <f t="shared" si="0"/>
+        <v>5.6588750000000001</v>
+      </c>
+      <c r="C24" s="11">
+        <f t="shared" si="1"/>
+        <v>32.022866265624998</v>
+      </c>
+      <c r="D24" s="10">
         <v>22.058</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="6">
+        <f t="shared" si="2"/>
+        <v>4.2083333333330586E-2</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="3"/>
+        <v>1.7710069444442133E-3</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="3">
-        <f>(24.05-16.2)/E21</f>
-        <v>6.5765749425686444</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="I24" s="3">
+        <f>(24.05-16.2)/I21</f>
+        <v>6.4381052253687825</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
         <v>16.004000000000001</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="13">
+        <f t="shared" si="0"/>
+        <v>1.9528750000000006</v>
+      </c>
+      <c r="C25" s="14">
+        <f t="shared" si="1"/>
+        <v>3.8137207656250021</v>
+      </c>
+      <c r="D25" s="12">
         <v>21.157</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="13">
+        <f t="shared" si="2"/>
+        <v>-0.85891666666666922</v>
+      </c>
+      <c r="F25" s="14">
+        <f t="shared" si="3"/>
+        <v>0.73773784027778211</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="3">
+      <c r="I25" s="3">
         <v>0.999</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D26" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="4">
-        <f>E24^2/(E24^2+E22)</f>
-        <v>0.48460156403738552</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="I26" s="4">
+        <f>I24^2/(I24^2+I22)</f>
+        <v>0.47398031563072685</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>